<commit_message>
Add 2015 post-harvest LIND visit data
- above-ground biomass areal mass density (field residue)
- crop height
</commit_message>
<xml_diff>
--- a/records/Sampling dates.xlsx
+++ b/records/Sampling dates.xlsx
@@ -10,9 +10,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$52</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -42,7 +42,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="m\/d"/>
+    <numFmt numFmtId="164" formatCode="m\/d"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -75,7 +75,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -98,31 +98,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -432,16 +484,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="7" customWidth="1"/>
-    <col min="2" max="6" width="15.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="5" customWidth="1"/>
+    <col min="2" max="6" width="15.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -465,512 +517,525 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="7">
         <v>2012</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>41047</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>41047</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4">
+      <c r="A3" s="7"/>
+      <c r="B3" s="3">
         <v>41064</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>41064</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="C4" s="4">
+      <c r="A4" s="7"/>
+      <c r="C4" s="3">
         <v>41081</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3">
         <v>41088</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="C6" s="4">
+      <c r="A6" s="7"/>
+      <c r="C6" s="3">
         <v>41103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4">
+      <c r="A7" s="7"/>
+      <c r="B7" s="3">
         <v>41138</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>41138</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4">
+      <c r="A8" s="7"/>
+      <c r="B8" s="3">
         <v>41173</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>41173</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="8">
         <v>2013</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4">
         <v>41408</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6">
+      <c r="A10" s="8"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4">
         <v>41422</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6">
+      <c r="A11" s="8"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4">
         <v>41435</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6">
+      <c r="A12" s="8"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4">
         <v>41454</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6">
+      <c r="A13" s="8"/>
+      <c r="B13" s="4">
         <v>41470</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4">
         <v>41470</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6">
+      <c r="A14" s="8"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4">
         <v>41476</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6">
+      <c r="A15" s="8"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4">
         <v>41484</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6">
+      <c r="A16" s="8"/>
+      <c r="B16" s="4">
         <v>41485</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6">
+      <c r="A17" s="8"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4">
         <v>41487</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6">
+      <c r="A18" s="8"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4">
         <v>41492</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6">
+      <c r="A19" s="8"/>
+      <c r="B19" s="4">
         <v>41516</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <v>41516</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="7">
         <v>2014</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>41773</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>41773</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4">
+      <c r="A21" s="7"/>
+      <c r="B21" s="3">
         <v>41788</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>41788</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4">
+      <c r="A22" s="7"/>
+      <c r="B22" s="3">
         <v>41801</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>41801</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="E23" s="4">
+      <c r="A23" s="7"/>
+      <c r="E23" s="3">
         <v>41813</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4">
+      <c r="A24" s="7"/>
+      <c r="B24" s="3">
         <v>41815</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>41815</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="E25" s="4">
+      <c r="A25" s="7"/>
+      <c r="E25" s="3">
         <v>41828</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4">
+      <c r="A26" s="7"/>
+      <c r="B26" s="3">
         <v>41835</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>41835</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="E27" s="4">
+      <c r="A27" s="7"/>
+      <c r="E27" s="3">
         <v>41844</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4">
+      <c r="A28" s="7"/>
+      <c r="B28" s="3">
         <v>41853</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>41853</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="E29" s="4">
+      <c r="A29" s="9"/>
+      <c r="E29" s="3">
         <v>41857</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="10">
         <v>2015</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4">
         <v>42082</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6">
+      <c r="A31" s="11"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4">
         <v>42090</v>
       </c>
-      <c r="F31" s="6"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6">
+      <c r="A32" s="11"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4">
         <v>42093</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6">
+      <c r="A33" s="11"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4">
         <v>42107</v>
       </c>
-      <c r="F33" s="6"/>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6">
+      <c r="A34" s="11"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4">
         <v>42108</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6">
+      <c r="A35" s="11"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4">
         <v>42121</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6">
+      <c r="A36" s="11"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4">
         <v>42122</v>
       </c>
-      <c r="F36" s="6"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6">
+      <c r="A37" s="11"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4">
         <v>42135</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6">
+      <c r="A38" s="11"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4">
         <v>42136</v>
       </c>
-      <c r="F38" s="6"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6">
+      <c r="A39" s="11"/>
+      <c r="B39" s="4">
         <v>42142</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="4">
         <v>42142</v>
       </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6">
+      <c r="A40" s="11"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4">
         <v>42150</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="4">
         <v>42150</v>
       </c>
-      <c r="F40" s="6"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6">
+      <c r="A41" s="11"/>
+      <c r="B41" s="4">
         <v>42156</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="4">
         <v>42156</v>
       </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6">
+      <c r="A42" s="11"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4">
         <v>42163</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="4">
         <v>42163</v>
       </c>
-      <c r="F42" s="6"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="6">
+      <c r="A43" s="11"/>
+      <c r="B43" s="4">
         <v>42170</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="4">
         <v>42170</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6">
+      <c r="A44" s="11"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4">
         <v>42177</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="4">
         <v>42177</v>
       </c>
-      <c r="F44" s="6"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6">
+      <c r="A45" s="11"/>
+      <c r="B45" s="4">
         <v>42184</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="4">
         <v>42184</v>
       </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6">
+      <c r="A46" s="11"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4">
         <v>42191</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="4">
         <v>42191</v>
       </c>
-      <c r="F46" s="6"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6">
+      <c r="A47" s="11"/>
+      <c r="B47" s="4">
         <v>42198</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="4">
         <v>42198</v>
       </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6">
+      <c r="A48" s="11"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4">
         <v>42205</v>
       </c>
-      <c r="F48" s="6"/>
+      <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="6">
+      <c r="A49" s="11"/>
+      <c r="B49" s="4">
         <v>42212</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="4">
         <v>42212</v>
       </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6">
+      <c r="A50" s="11"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4">
         <v>42219</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="4">
         <v>42219</v>
       </c>
-      <c r="F50" s="6"/>
+      <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6">
+      <c r="A51" s="11"/>
+      <c r="B51" s="4">
         <v>42226</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C51" s="4">
         <v>42226</v>
       </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4">
+        <v>42261</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A19"/>
     <mergeCell ref="A20:A29"/>
-    <mergeCell ref="A30:A51"/>
+    <mergeCell ref="A30:A52"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="92" fitToWidth="0" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="90" fitToWidth="0" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add data from 1st events at CFNT, CFCT
</commit_message>
<xml_diff>
--- a/records/Sampling dates.xlsx
+++ b/records/Sampling dates.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m\/d"/>
   </numFmts>
@@ -139,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,25 +156,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -484,10 +487,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +521,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>2012</v>
       </c>
       <c r="B2" s="3">
@@ -528,7 +532,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="3">
         <v>41064</v>
       </c>
@@ -537,25 +541,25 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="C4" s="3">
         <v>41081</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="3">
         <v>41088</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="C6" s="3">
         <v>41103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="3">
         <v>41138</v>
       </c>
@@ -564,7 +568,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="3">
         <v>41173</v>
       </c>
@@ -573,7 +577,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>2013</v>
       </c>
       <c r="B9" s="4"/>
@@ -585,7 +589,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4">
@@ -595,7 +599,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4">
@@ -605,7 +609,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4">
@@ -615,7 +619,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="4">
         <v>41470</v>
       </c>
@@ -627,7 +631,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4">
@@ -637,7 +641,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -647,7 +651,7 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="4">
         <v>41485</v>
       </c>
@@ -657,7 +661,7 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4">
@@ -667,7 +671,7 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -677,7 +681,7 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="4">
         <v>41516</v>
       </c>
@@ -689,7 +693,7 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>2014</v>
       </c>
       <c r="B20" s="3">
@@ -700,7 +704,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="3">
         <v>41788</v>
       </c>
@@ -709,7 +713,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="3">
         <v>41801</v>
       </c>
@@ -718,13 +722,13 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="6"/>
       <c r="E23" s="3">
         <v>41813</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="3">
         <v>41815</v>
       </c>
@@ -733,13 +737,13 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
       <c r="E25" s="3">
         <v>41828</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6"/>
       <c r="B26" s="3">
         <v>41835</v>
       </c>
@@ -748,13 +752,13 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6"/>
       <c r="E27" s="3">
         <v>41844</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="6"/>
       <c r="B28" s="3">
         <v>41853</v>
       </c>
@@ -763,13 +767,13 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="8"/>
       <c r="E29" s="3">
         <v>41857</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+      <c r="A30" s="9">
         <v>2015</v>
       </c>
       <c r="B30" s="4"/>
@@ -781,7 +785,7 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -791,7 +795,7 @@
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4">
@@ -801,7 +805,7 @@
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -811,7 +815,7 @@
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4">
@@ -821,7 +825,7 @@
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4">
@@ -831,7 +835,7 @@
       <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -841,7 +845,7 @@
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4">
@@ -851,7 +855,7 @@
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -861,7 +865,7 @@
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="4">
         <v>42142</v>
       </c>
@@ -873,7 +877,7 @@
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4">
@@ -885,7 +889,7 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="4">
         <v>42156</v>
       </c>
@@ -897,7 +901,7 @@
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4">
@@ -909,7 +913,7 @@
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="4">
         <v>42170</v>
       </c>
@@ -921,7 +925,7 @@
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4">
@@ -933,7 +937,7 @@
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="4">
         <v>42184</v>
       </c>
@@ -945,7 +949,7 @@
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4">
@@ -957,7 +961,7 @@
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="4">
         <v>42198</v>
       </c>
@@ -969,7 +973,7 @@
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -979,7 +983,7 @@
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="4">
         <v>42212</v>
       </c>
@@ -991,7 +995,7 @@
       <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
+      <c r="A50" s="10"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4">
@@ -1003,7 +1007,7 @@
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
+      <c r="A51" s="10"/>
       <c r="B51" s="4">
         <v>42226</v>
       </c>
@@ -1015,7 +1019,7 @@
       <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4">
@@ -1025,14 +1029,56 @@
       <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
+      <c r="A53" s="8">
+        <v>2016</v>
+      </c>
+      <c r="B53" s="3">
+        <v>42480</v>
+      </c>
+      <c r="C53" s="3">
+        <v>42480</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A19"/>
     <mergeCell ref="A20:A29"/>
     <mergeCell ref="A30:A52"/>
+    <mergeCell ref="A53:A64"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish data entry for crop year 2016
</commit_message>
<xml_diff>
--- a/records/Sampling dates.xlsx
+++ b/records/Sampling dates.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$52</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Year</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>MMTN</t>
-  </si>
-  <si>
-    <t>MSLK</t>
   </si>
   <si>
     <t>CFCT (Clark)</t>
@@ -40,7 +37,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m\/d"/>
   </numFmts>
@@ -139,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,6 +153,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -174,10 +174,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,28 +487,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="5" customWidth="1"/>
-    <col min="2" max="6" width="15.7109375" style="3" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -516,12 +516,9 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>2012</v>
       </c>
       <c r="B2" s="3">
@@ -531,8 +528,8 @@
         <v>41047</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
       <c r="B3" s="3">
         <v>41064</v>
       </c>
@@ -540,26 +537,26 @@
         <v>41064</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
       <c r="C4" s="3">
         <v>41081</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
       <c r="B5" s="3">
         <v>41088</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
       <c r="C6" s="3">
         <v>41103</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
       <c r="B7" s="3">
         <v>41138</v>
       </c>
@@ -567,8 +564,8 @@
         <v>41138</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
       <c r="B8" s="3">
         <v>41173</v>
       </c>
@@ -576,8 +573,8 @@
         <v>41173</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>2013</v>
       </c>
       <c r="B9" s="4"/>
@@ -586,40 +583,36 @@
         <v>41408</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4">
         <v>41422</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4">
         <v>41435</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4">
         <v>41454</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
       <c r="B13" s="4">
         <v>41470</v>
       </c>
@@ -628,60 +621,54 @@
       <c r="E13" s="4">
         <v>41470</v>
       </c>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4">
         <v>41476</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4">
         <v>41484</v>
       </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
       <c r="B16" s="4">
         <v>41485</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4">
         <v>41487</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4">
         <v>41492</v>
       </c>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
       <c r="B19" s="4">
         <v>41516</v>
       </c>
@@ -690,10 +677,9 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>2014</v>
       </c>
       <c r="B20" s="3">
@@ -703,8 +689,8 @@
         <v>41773</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
       <c r="B21" s="3">
         <v>41788</v>
       </c>
@@ -712,8 +698,8 @@
         <v>41788</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
       <c r="B22" s="3">
         <v>41801</v>
       </c>
@@ -721,14 +707,14 @@
         <v>41801</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
       <c r="E23" s="3">
         <v>41813</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
       <c r="B24" s="3">
         <v>41815</v>
       </c>
@@ -736,14 +722,14 @@
         <v>41815</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
       <c r="E25" s="3">
         <v>41828</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
       <c r="B26" s="3">
         <v>41835</v>
       </c>
@@ -751,14 +737,14 @@
         <v>41835</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
       <c r="E27" s="3">
         <v>41844</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
       <c r="B28" s="3">
         <v>41853</v>
       </c>
@@ -766,14 +752,14 @@
         <v>41853</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
       <c r="E29" s="3">
         <v>41857</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
         <v>2015</v>
       </c>
       <c r="B30" s="4"/>
@@ -782,90 +768,81 @@
         <v>42082</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4">
         <v>42090</v>
       </c>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4">
         <v>42093</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4">
         <v>42107</v>
       </c>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4">
         <v>42108</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4">
         <v>42121</v>
       </c>
       <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4">
         <v>42122</v>
       </c>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4">
         <v>42135</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4">
         <v>42136</v>
       </c>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
       <c r="B39" s="4">
         <v>42142</v>
       </c>
@@ -874,10 +851,9 @@
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4">
@@ -886,10 +862,9 @@
       <c r="E40" s="4">
         <v>42150</v>
       </c>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
       <c r="B41" s="4">
         <v>42156</v>
       </c>
@@ -898,10 +873,9 @@
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4">
@@ -910,10 +884,9 @@
       <c r="E42" s="4">
         <v>42163</v>
       </c>
-      <c r="F42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
       <c r="B43" s="4">
         <v>42170</v>
       </c>
@@ -922,10 +895,9 @@
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4">
@@ -934,10 +906,9 @@
       <c r="E44" s="4">
         <v>42177</v>
       </c>
-      <c r="F44" s="4"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
       <c r="B45" s="4">
         <v>42184</v>
       </c>
@@ -946,10 +917,9 @@
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4">
@@ -958,10 +928,9 @@
       <c r="E46" s="4">
         <v>42191</v>
       </c>
-      <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
       <c r="B47" s="4">
         <v>42198</v>
       </c>
@@ -970,20 +939,18 @@
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4">
         <v>42205</v>
       </c>
-      <c r="F48" s="4"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
       <c r="B49" s="4">
         <v>42212</v>
       </c>
@@ -992,10 +959,9 @@
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4">
@@ -1004,10 +970,9 @@
       <c r="E50" s="4">
         <v>42219</v>
       </c>
-      <c r="F50" s="4"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
       <c r="B51" s="4">
         <v>42226</v>
       </c>
@@ -1016,20 +981,18 @@
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4">
         <v>42261</v>
       </c>
       <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="8">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="9">
         <v>2016</v>
       </c>
       <c r="B53" s="3">
@@ -1039,38 +1002,116 @@
         <v>42480</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="3">
+        <v>42858</v>
+      </c>
+      <c r="C54" s="3">
+        <v>42858</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="3">
+        <v>42869</v>
+      </c>
+      <c r="C55" s="3">
+        <v>42869</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="3">
+        <v>42881</v>
+      </c>
+      <c r="C56" s="3">
+        <v>42881</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="3">
+        <v>42894</v>
+      </c>
+      <c r="C57" s="3">
+        <v>42894</v>
+      </c>
+      <c r="E57" s="3">
+        <v>42894</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E58" s="3">
+        <v>42903</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="3">
+        <v>42908</v>
+      </c>
+      <c r="C59" s="3">
+        <v>42908</v>
+      </c>
+      <c r="E59" s="3">
+        <v>42908</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="3">
+        <v>42922</v>
+      </c>
+      <c r="C60" s="3">
+        <v>42922</v>
+      </c>
+      <c r="E60" s="3">
+        <v>42922</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E61" s="3">
+        <v>42936</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="3">
+        <v>42943</v>
+      </c>
+      <c r="C62" s="3">
+        <v>42943</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
+      <c r="B63" s="3">
+        <v>42950</v>
+      </c>
+      <c r="C63" s="3">
+        <v>42950</v>
+      </c>
+      <c r="E63" s="3">
+        <v>42950</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="E64" s="3">
+        <v>42964</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="E65" s="3">
+        <v>42973</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1078,7 +1119,7 @@
     <mergeCell ref="A9:A19"/>
     <mergeCell ref="A20:A29"/>
     <mergeCell ref="A30:A52"/>
-    <mergeCell ref="A53:A64"/>
+    <mergeCell ref="A53:A65"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>